<commit_message>
Backup to GitHub - 2021.03.30
</commit_message>
<xml_diff>
--- a/01_Linear_Regression/Output/PetrolCon_00_Results_Summary.xlsx
+++ b/01_Linear_Regression/Output/PetrolCon_00_Results_Summary.xlsx
@@ -12,13 +12,14 @@
     <sheet name="PCA_VAR" sheetId="3" r:id="rId3"/>
     <sheet name="PCA_Components" sheetId="4" r:id="rId4"/>
     <sheet name="PCA_Top_Features" sheetId="5" r:id="rId5"/>
+    <sheet name="DTR-Features" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>count</t>
   </si>
@@ -93,6 +94,24 @@
   </si>
   <si>
     <t>weak</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>0.384</t>
+  </si>
+  <si>
+    <t>0.303</t>
+  </si>
+  <si>
+    <t>0.163</t>
+  </si>
+  <si>
+    <t>0.15</t>
   </si>
 </sst>
 </file>
@@ -963,4 +982,69 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Backup to GitHub - 2021.04.11
</commit_message>
<xml_diff>
--- a/01_Linear_Regression/Output/PetrolCon_00_Results_Summary.xlsx
+++ b/01_Linear_Regression/Output/PetrolCon_00_Results_Summary.xlsx
@@ -745,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.395</v>
+        <v>0.371</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -753,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.286</v>
+        <v>0.322</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -761,7 +761,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.229</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -769,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.09</v>
+        <v>0.077</v>
       </c>
     </row>
   </sheetData>
@@ -804,16 +804,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-0.71</v>
+        <v>-0.271</v>
       </c>
       <c r="C2">
-        <v>0.124</v>
+        <v>0.858</v>
       </c>
       <c r="D2">
-        <v>0.615</v>
+        <v>0.249</v>
       </c>
       <c r="E2">
-        <v>0.319</v>
+        <v>0.357</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -821,16 +821,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.081</v>
+        <v>-0.635</v>
       </c>
       <c r="C3">
-        <v>0.617</v>
+        <v>-0.431</v>
       </c>
       <c r="D3">
-        <v>-0.384</v>
+        <v>0.631</v>
       </c>
       <c r="E3">
-        <v>0.6820000000000001</v>
+        <v>0.114</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -838,16 +838,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.19</v>
+        <v>0.116</v>
       </c>
       <c r="C4">
-        <v>0.76</v>
+        <v>0.259</v>
       </c>
       <c r="D4">
-        <v>0.336</v>
+        <v>0.448</v>
       </c>
       <c r="E4">
-        <v>-0.522</v>
+        <v>-0.848</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -855,16 +855,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.673</v>
+        <v>0.714</v>
       </c>
       <c r="C5">
-        <v>-0.159</v>
+        <v>-0.1</v>
       </c>
       <c r="D5">
-        <v>0.601</v>
+        <v>0.583</v>
       </c>
       <c r="E5">
-        <v>0.401</v>
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Backup to GitHub - 2021.04.18
</commit_message>
<xml_diff>
--- a/01_Linear_Regression/Output/PetrolCon_00_Results_Summary.xlsx
+++ b/01_Linear_Regression/Output/PetrolCon_00_Results_Summary.xlsx
@@ -7,19 +7,47 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Stats" sheetId="1" r:id="rId1"/>
-    <sheet name="VIF" sheetId="2" r:id="rId2"/>
-    <sheet name="PCA_VAR" sheetId="3" r:id="rId3"/>
-    <sheet name="PCA_Components" sheetId="4" r:id="rId4"/>
-    <sheet name="PCA_Top_Features" sheetId="5" r:id="rId5"/>
-    <sheet name="DTR-Features" sheetId="6" r:id="rId6"/>
+    <sheet name="Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Stats" sheetId="2" r:id="rId2"/>
+    <sheet name="VIF" sheetId="3" r:id="rId3"/>
+    <sheet name="PCA_VAR" sheetId="4" r:id="rId4"/>
+    <sheet name="PCA_Components" sheetId="5" r:id="rId5"/>
+    <sheet name="PCA_Top_Features" sheetId="6" r:id="rId6"/>
+    <sheet name="DTR-Features" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Petrol_tax</t>
+  </si>
+  <si>
+    <t>Average_income</t>
+  </si>
+  <si>
+    <t>Paved_Highways</t>
+  </si>
+  <si>
+    <t>Population_Driver_licence(%)</t>
+  </si>
+  <si>
+    <t>Petrol_Consumption</t>
+  </si>
+  <si>
+    <t>float64</t>
+  </si>
+  <si>
+    <t>int64</t>
+  </si>
   <si>
     <t>count</t>
   </si>
@@ -43,21 +71,6 @@
   </si>
   <si>
     <t>max</t>
-  </si>
-  <si>
-    <t>Petrol_tax</t>
-  </si>
-  <si>
-    <t>Average_income</t>
-  </si>
-  <si>
-    <t>Paved_Highways</t>
-  </si>
-  <si>
-    <t>Population_Driver_licence(%)</t>
-  </si>
-  <si>
-    <t>Petrol_Consumption</t>
   </si>
   <si>
     <t>Feature</t>
@@ -469,181 +482,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
+      <c r="C6" t="s">
         <v>8</v>
-      </c>
-      <c r="B2">
-        <v>48</v>
-      </c>
-      <c r="C2">
-        <v>7.668</v>
-      </c>
-      <c r="D2">
-        <v>0.951</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-      <c r="G2">
-        <v>7.5</v>
-      </c>
-      <c r="H2">
-        <v>8.125</v>
-      </c>
-      <c r="I2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>48</v>
-      </c>
-      <c r="C3">
-        <v>4241.833</v>
-      </c>
-      <c r="D3">
-        <v>573.624</v>
-      </c>
-      <c r="E3">
-        <v>3063</v>
-      </c>
-      <c r="F3">
-        <v>3739</v>
-      </c>
-      <c r="G3">
-        <v>4298</v>
-      </c>
-      <c r="H3">
-        <v>4578.75</v>
-      </c>
-      <c r="I3">
-        <v>5342</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>48</v>
-      </c>
-      <c r="C4">
-        <v>5565.417</v>
-      </c>
-      <c r="D4">
-        <v>3491.507</v>
-      </c>
-      <c r="E4">
-        <v>431</v>
-      </c>
-      <c r="F4">
-        <v>3110.25</v>
-      </c>
-      <c r="G4">
-        <v>4735.5</v>
-      </c>
-      <c r="H4">
-        <v>7156</v>
-      </c>
-      <c r="I4">
-        <v>17782</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>48</v>
-      </c>
-      <c r="C5">
-        <v>0.57</v>
-      </c>
-      <c r="D5">
-        <v>0.055</v>
-      </c>
-      <c r="E5">
-        <v>0.451</v>
-      </c>
-      <c r="F5">
-        <v>0.53</v>
-      </c>
-      <c r="G5">
-        <v>0.5639999999999999</v>
-      </c>
-      <c r="H5">
-        <v>0.595</v>
-      </c>
-      <c r="I5">
-        <v>0.724</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>48</v>
-      </c>
-      <c r="C6">
-        <v>576.771</v>
-      </c>
-      <c r="D6">
-        <v>111.886</v>
-      </c>
-      <c r="E6">
-        <v>344</v>
-      </c>
-      <c r="F6">
-        <v>509.5</v>
-      </c>
-      <c r="G6">
-        <v>568.5</v>
-      </c>
-      <c r="H6">
-        <v>632.75</v>
-      </c>
-      <c r="I6">
-        <v>968</v>
       </c>
     </row>
   </sheetData>
@@ -652,6 +557,190 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>48</v>
+      </c>
+      <c r="C2">
+        <v>7.668</v>
+      </c>
+      <c r="D2">
+        <v>0.951</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>7.5</v>
+      </c>
+      <c r="H2">
+        <v>8.125</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>4241.833</v>
+      </c>
+      <c r="D3">
+        <v>573.624</v>
+      </c>
+      <c r="E3">
+        <v>3063</v>
+      </c>
+      <c r="F3">
+        <v>3739</v>
+      </c>
+      <c r="G3">
+        <v>4298</v>
+      </c>
+      <c r="H3">
+        <v>4578.75</v>
+      </c>
+      <c r="I3">
+        <v>5342</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>5565.417</v>
+      </c>
+      <c r="D4">
+        <v>3491.507</v>
+      </c>
+      <c r="E4">
+        <v>431</v>
+      </c>
+      <c r="F4">
+        <v>3110.25</v>
+      </c>
+      <c r="G4">
+        <v>4735.5</v>
+      </c>
+      <c r="H4">
+        <v>7156</v>
+      </c>
+      <c r="I4">
+        <v>17782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>0.57</v>
+      </c>
+      <c r="D5">
+        <v>0.055</v>
+      </c>
+      <c r="E5">
+        <v>0.451</v>
+      </c>
+      <c r="F5">
+        <v>0.53</v>
+      </c>
+      <c r="G5">
+        <v>0.5639999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.595</v>
+      </c>
+      <c r="I5">
+        <v>0.724</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>576.771</v>
+      </c>
+      <c r="D6">
+        <v>111.886</v>
+      </c>
+      <c r="E6">
+        <v>344</v>
+      </c>
+      <c r="F6">
+        <v>509.5</v>
+      </c>
+      <c r="G6">
+        <v>568.5</v>
+      </c>
+      <c r="H6">
+        <v>632.75</v>
+      </c>
+      <c r="I6">
+        <v>968</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -661,10 +750,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -672,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>45.86828470683663</v>
@@ -683,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>71.75766085533557</v>
@@ -694,7 +783,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>3.902246686799693</v>
@@ -705,7 +794,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>259.6466665406508</v>
@@ -716,7 +805,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>79.89342086234312</v>
@@ -727,7 +816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -777,7 +866,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -872,7 +961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -882,16 +971,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -899,16 +988,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>-0.71</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -916,16 +1005,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>0.6820000000000001</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -933,16 +1022,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>0.76</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -950,16 +1039,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D5">
         <v>0.673</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -967,16 +1056,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>0.615</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +1073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -994,10 +1083,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1005,10 +1094,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1016,10 +1105,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1027,10 +1116,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1038,10 +1127,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>